<commit_message>
Fixed strings in workbooks, make script for producing regional mega tables
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/regions/InputForCode_Kaskazini_Pemba.xlsx
+++ b/input_spreadsheets/Tanzania/regions/InputForCode_Kaskazini_Pemba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Tanzania/regions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{08B103D9-646B-3B4F-B3F4-889BA3BFE028}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{E7908ABF-B2FE-EC47-8CD3-4CEA6AAF41CE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23320" windowHeight="15540" tabRatio="905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15540" tabRatio="905" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expenditure &amp; budget" sheetId="47" r:id="rId1"/>
@@ -4137,7 +4137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="275">
   <si>
     <t>year</t>
   </si>
@@ -4952,9 +4952,6 @@
     <t>under 5</t>
   </si>
   <si>
-    <t>Not used/needed</t>
-  </si>
-  <si>
     <t>Kangaroo mother care</t>
   </si>
   <si>
@@ -6425,13 +6422,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="739" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="739" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="739" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="741">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
@@ -8800,36 +8797,36 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.5" style="158" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" style="158" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="158"/>
+    <col min="1" max="1" width="17.5" style="157" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" style="157" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="157"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" s="157" t="s">
+      <c r="A1" s="156" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="157" t="s">
+      <c r="B1" s="156" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" s="156" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" s="157" t="s">
+      <c r="B2" s="158"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" s="156" t="s">
         <v>274</v>
       </c>
-      <c r="B2" s="159"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" s="157" t="s">
-        <v>275</v>
-      </c>
-      <c r="B3" s="160"/>
+      <c r="B3" s="159"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13782,7 +13779,7 @@
         <v>233</v>
       </c>
       <c r="B18" s="152" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C18" s="153">
         <v>1.5</v>
@@ -13927,7 +13924,7 @@
       <c r="A2" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="B2" s="156" t="s">
+      <c r="B2" s="160" t="s">
         <v>72</v>
       </c>
       <c r="C2" t="s">
@@ -13950,7 +13947,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B3" s="156"/>
+      <c r="B3" s="160"/>
       <c r="C3" t="s">
         <v>150</v>
       </c>
@@ -13972,7 +13969,7 @@
       <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B4" s="156"/>
+      <c r="B4" s="160"/>
       <c r="C4" t="s">
         <v>160</v>
       </c>
@@ -13994,7 +13991,7 @@
       <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B5" s="156" t="s">
+      <c r="B5" s="160" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
@@ -14017,7 +14014,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B6" s="156"/>
+      <c r="B6" s="160"/>
       <c r="C6" t="s">
         <v>150</v>
       </c>
@@ -14038,7 +14035,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B7" s="156"/>
+      <c r="B7" s="160"/>
       <c r="C7" t="s">
         <v>160</v>
       </c>
@@ -14059,7 +14056,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B8" s="156" t="s">
+      <c r="B8" s="160" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
@@ -14082,7 +14079,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B9" s="156"/>
+      <c r="B9" s="160"/>
       <c r="C9" t="s">
         <v>150</v>
       </c>
@@ -14103,7 +14100,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B10" s="156"/>
+      <c r="B10" s="160"/>
       <c r="C10" t="s">
         <v>160</v>
       </c>
@@ -14124,7 +14121,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B11" s="156" t="s">
+      <c r="B11" s="160" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
@@ -14147,7 +14144,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B12" s="156"/>
+      <c r="B12" s="160"/>
       <c r="C12" t="s">
         <v>150</v>
       </c>
@@ -14168,7 +14165,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B13" s="156"/>
+      <c r="B13" s="160"/>
       <c r="C13" t="s">
         <v>160</v>
       </c>
@@ -14189,7 +14186,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B14" s="156" t="s">
+      <c r="B14" s="160" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
@@ -14212,7 +14209,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B15" s="156"/>
+      <c r="B15" s="160"/>
       <c r="C15" t="s">
         <v>150</v>
       </c>
@@ -14233,7 +14230,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B16" s="156"/>
+      <c r="B16" s="160"/>
       <c r="C16" t="s">
         <v>160</v>
       </c>
@@ -14287,7 +14284,7 @@
       <c r="A19" s="42" t="s">
         <v>154</v>
       </c>
-      <c r="B19" s="156" t="s">
+      <c r="B19" s="160" t="s">
         <v>72</v>
       </c>
       <c r="C19" t="s">
@@ -14310,7 +14307,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B20" s="156"/>
+      <c r="B20" s="160"/>
       <c r="C20" t="s">
         <v>150</v>
       </c>
@@ -14331,7 +14328,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B21" s="156"/>
+      <c r="B21" s="160"/>
       <c r="C21" t="s">
         <v>160</v>
       </c>
@@ -14352,7 +14349,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B22" s="156" t="s">
+      <c r="B22" s="160" t="s">
         <v>6</v>
       </c>
       <c r="C22" t="s">
@@ -14375,7 +14372,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B23" s="156"/>
+      <c r="B23" s="160"/>
       <c r="C23" t="s">
         <v>150</v>
       </c>
@@ -14396,7 +14393,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B24" s="156"/>
+      <c r="B24" s="160"/>
       <c r="C24" t="s">
         <v>160</v>
       </c>
@@ -14417,7 +14414,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B25" s="156" t="s">
+      <c r="B25" s="160" t="s">
         <v>7</v>
       </c>
       <c r="C25" t="s">
@@ -14440,7 +14437,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B26" s="156"/>
+      <c r="B26" s="160"/>
       <c r="C26" t="s">
         <v>150</v>
       </c>
@@ -14461,7 +14458,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B27" s="156"/>
+      <c r="B27" s="160"/>
       <c r="C27" t="s">
         <v>160</v>
       </c>
@@ -14482,7 +14479,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B28" s="156" t="s">
+      <c r="B28" s="160" t="s">
         <v>8</v>
       </c>
       <c r="C28" t="s">
@@ -14505,7 +14502,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B29" s="156"/>
+      <c r="B29" s="160"/>
       <c r="C29" t="s">
         <v>150</v>
       </c>
@@ -14526,7 +14523,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B30" s="156"/>
+      <c r="B30" s="160"/>
       <c r="C30" t="s">
         <v>160</v>
       </c>
@@ -14547,7 +14544,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B31" s="156" t="s">
+      <c r="B31" s="160" t="s">
         <v>9</v>
       </c>
       <c r="C31" t="s">
@@ -14570,7 +14567,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B32" s="156"/>
+      <c r="B32" s="160"/>
       <c r="C32" t="s">
         <v>150</v>
       </c>
@@ -14591,7 +14588,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B33" s="156"/>
+      <c r="B33" s="160"/>
       <c r="C33" t="s">
         <v>160</v>
       </c>
@@ -14638,7 +14635,7 @@
       <c r="A36" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="B36" s="156" t="s">
+      <c r="B36" s="160" t="s">
         <v>72</v>
       </c>
       <c r="C36" t="s">
@@ -14661,7 +14658,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B37" s="156"/>
+      <c r="B37" s="160"/>
       <c r="C37" t="s">
         <v>150</v>
       </c>
@@ -14682,7 +14679,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B38" s="156"/>
+      <c r="B38" s="160"/>
       <c r="C38" t="s">
         <v>160</v>
       </c>
@@ -14704,7 +14701,7 @@
       <c r="I38" s="38"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B39" s="156" t="s">
+      <c r="B39" s="160" t="s">
         <v>6</v>
       </c>
       <c r="C39" t="s">
@@ -14727,7 +14724,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B40" s="156"/>
+      <c r="B40" s="160"/>
       <c r="C40" t="s">
         <v>150</v>
       </c>
@@ -14748,7 +14745,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B41" s="156"/>
+      <c r="B41" s="160"/>
       <c r="C41" t="s">
         <v>160</v>
       </c>
@@ -14769,7 +14766,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B42" s="156" t="s">
+      <c r="B42" s="160" t="s">
         <v>7</v>
       </c>
       <c r="C42" t="s">
@@ -14792,7 +14789,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B43" s="156"/>
+      <c r="B43" s="160"/>
       <c r="C43" t="s">
         <v>150</v>
       </c>
@@ -14813,7 +14810,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B44" s="156"/>
+      <c r="B44" s="160"/>
       <c r="C44" t="s">
         <v>160</v>
       </c>
@@ -14834,7 +14831,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B45" s="156" t="s">
+      <c r="B45" s="160" t="s">
         <v>8</v>
       </c>
       <c r="C45" t="s">
@@ -14857,7 +14854,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B46" s="156"/>
+      <c r="B46" s="160"/>
       <c r="C46" t="s">
         <v>150</v>
       </c>
@@ -14878,7 +14875,7 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B47" s="156"/>
+      <c r="B47" s="160"/>
       <c r="C47" t="s">
         <v>160</v>
       </c>
@@ -14899,7 +14896,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B48" s="156" t="s">
+      <c r="B48" s="160" t="s">
         <v>9</v>
       </c>
       <c r="C48" t="s">
@@ -14922,7 +14919,7 @@
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B49" s="156"/>
+      <c r="B49" s="160"/>
       <c r="C49" t="s">
         <v>150</v>
       </c>
@@ -14943,7 +14940,7 @@
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B50" s="156"/>
+      <c r="B50" s="160"/>
       <c r="C50" t="s">
         <v>160</v>
       </c>
@@ -14988,11 +14985,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -15003,6 +14995,11 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -18912,7 +18909,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A53" s="152" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B53" s="152" t="s">
         <v>21</v>
@@ -20023,7 +20020,7 @@
     <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="152"/>
       <c r="B14" s="152" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C14" s="109">
         <v>1</v>
@@ -22451,7 +22448,7 @@
     <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A14" s="152"/>
       <c r="B14" s="152" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C14" s="109">
         <v>1</v>
@@ -24565,7 +24562,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" s="152" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -25112,7 +25109,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A52" s="152" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B52" s="152"/>
       <c r="C52" s="152"/>
@@ -26168,7 +26165,7 @@
     </row>
     <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="152" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B52" s="154">
         <v>0</v>
@@ -27869,7 +27866,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A102" s="152" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B102" s="152" t="s">
         <v>254</v>
@@ -27878,7 +27875,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A103" s="152" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B103" s="152" t="s">
         <v>255</v>
@@ -28294,7 +28291,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A52" s="152" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B52" s="152" t="s">
         <v>161</v>
@@ -30025,8 +30022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:O7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -30182,12 +30179,8 @@
     <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
-      <c r="C4" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>271</v>
-      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>

</xml_diff>

<commit_message>
Made up some current expenditures for regions (placeholder)
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/regions/InputForCode_Kaskazini_Pemba.xlsx
+++ b/input_spreadsheets/Tanzania/regions/InputForCode_Kaskazini_Pemba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Tanzania/regions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{E7908ABF-B2FE-EC47-8CD3-4CEA6AAF41CE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{95545FE7-8941-4B4F-A69B-31A00933A2F0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15540" tabRatio="905" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="15540" tabRatio="905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expenditure &amp; budget" sheetId="47" r:id="rId1"/>
@@ -6424,11 +6424,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="739" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="739" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="739" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="741">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
@@ -8797,7 +8797,7 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -8820,13 +8820,15 @@
       <c r="A2" s="156" t="s">
         <v>273</v>
       </c>
-      <c r="B2" s="158"/>
+      <c r="B2" s="160">
+        <v>65000</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="156" t="s">
         <v>274</v>
       </c>
-      <c r="B3" s="159"/>
+      <c r="B3" s="158"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13924,7 +13926,7 @@
       <c r="A2" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="B2" s="160" t="s">
+      <c r="B2" s="159" t="s">
         <v>72</v>
       </c>
       <c r="C2" t="s">
@@ -13947,7 +13949,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B3" s="160"/>
+      <c r="B3" s="159"/>
       <c r="C3" t="s">
         <v>150</v>
       </c>
@@ -13969,7 +13971,7 @@
       <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B4" s="160"/>
+      <c r="B4" s="159"/>
       <c r="C4" t="s">
         <v>160</v>
       </c>
@@ -13991,7 +13993,7 @@
       <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B5" s="160" t="s">
+      <c r="B5" s="159" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
@@ -14014,7 +14016,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B6" s="160"/>
+      <c r="B6" s="159"/>
       <c r="C6" t="s">
         <v>150</v>
       </c>
@@ -14035,7 +14037,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B7" s="160"/>
+      <c r="B7" s="159"/>
       <c r="C7" t="s">
         <v>160</v>
       </c>
@@ -14056,7 +14058,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B8" s="160" t="s">
+      <c r="B8" s="159" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
@@ -14079,7 +14081,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B9" s="160"/>
+      <c r="B9" s="159"/>
       <c r="C9" t="s">
         <v>150</v>
       </c>
@@ -14100,7 +14102,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B10" s="160"/>
+      <c r="B10" s="159"/>
       <c r="C10" t="s">
         <v>160</v>
       </c>
@@ -14121,7 +14123,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B11" s="160" t="s">
+      <c r="B11" s="159" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
@@ -14144,7 +14146,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B12" s="160"/>
+      <c r="B12" s="159"/>
       <c r="C12" t="s">
         <v>150</v>
       </c>
@@ -14165,7 +14167,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B13" s="160"/>
+      <c r="B13" s="159"/>
       <c r="C13" t="s">
         <v>160</v>
       </c>
@@ -14186,7 +14188,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B14" s="160" t="s">
+      <c r="B14" s="159" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
@@ -14209,7 +14211,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B15" s="160"/>
+      <c r="B15" s="159"/>
       <c r="C15" t="s">
         <v>150</v>
       </c>
@@ -14230,7 +14232,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B16" s="160"/>
+      <c r="B16" s="159"/>
       <c r="C16" t="s">
         <v>160</v>
       </c>
@@ -14284,7 +14286,7 @@
       <c r="A19" s="42" t="s">
         <v>154</v>
       </c>
-      <c r="B19" s="160" t="s">
+      <c r="B19" s="159" t="s">
         <v>72</v>
       </c>
       <c r="C19" t="s">
@@ -14307,7 +14309,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B20" s="160"/>
+      <c r="B20" s="159"/>
       <c r="C20" t="s">
         <v>150</v>
       </c>
@@ -14328,7 +14330,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B21" s="160"/>
+      <c r="B21" s="159"/>
       <c r="C21" t="s">
         <v>160</v>
       </c>
@@ -14349,7 +14351,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B22" s="160" t="s">
+      <c r="B22" s="159" t="s">
         <v>6</v>
       </c>
       <c r="C22" t="s">
@@ -14372,7 +14374,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B23" s="160"/>
+      <c r="B23" s="159"/>
       <c r="C23" t="s">
         <v>150</v>
       </c>
@@ -14393,7 +14395,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B24" s="160"/>
+      <c r="B24" s="159"/>
       <c r="C24" t="s">
         <v>160</v>
       </c>
@@ -14414,7 +14416,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B25" s="160" t="s">
+      <c r="B25" s="159" t="s">
         <v>7</v>
       </c>
       <c r="C25" t="s">
@@ -14437,7 +14439,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B26" s="160"/>
+      <c r="B26" s="159"/>
       <c r="C26" t="s">
         <v>150</v>
       </c>
@@ -14458,7 +14460,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B27" s="160"/>
+      <c r="B27" s="159"/>
       <c r="C27" t="s">
         <v>160</v>
       </c>
@@ -14479,7 +14481,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B28" s="160" t="s">
+      <c r="B28" s="159" t="s">
         <v>8</v>
       </c>
       <c r="C28" t="s">
@@ -14502,7 +14504,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B29" s="160"/>
+      <c r="B29" s="159"/>
       <c r="C29" t="s">
         <v>150</v>
       </c>
@@ -14523,7 +14525,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B30" s="160"/>
+      <c r="B30" s="159"/>
       <c r="C30" t="s">
         <v>160</v>
       </c>
@@ -14544,7 +14546,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B31" s="160" t="s">
+      <c r="B31" s="159" t="s">
         <v>9</v>
       </c>
       <c r="C31" t="s">
@@ -14567,7 +14569,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B32" s="160"/>
+      <c r="B32" s="159"/>
       <c r="C32" t="s">
         <v>150</v>
       </c>
@@ -14588,7 +14590,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B33" s="160"/>
+      <c r="B33" s="159"/>
       <c r="C33" t="s">
         <v>160</v>
       </c>
@@ -14635,7 +14637,7 @@
       <c r="A36" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="B36" s="160" t="s">
+      <c r="B36" s="159" t="s">
         <v>72</v>
       </c>
       <c r="C36" t="s">
@@ -14658,7 +14660,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B37" s="160"/>
+      <c r="B37" s="159"/>
       <c r="C37" t="s">
         <v>150</v>
       </c>
@@ -14679,7 +14681,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B38" s="160"/>
+      <c r="B38" s="159"/>
       <c r="C38" t="s">
         <v>160</v>
       </c>
@@ -14701,7 +14703,7 @@
       <c r="I38" s="38"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B39" s="160" t="s">
+      <c r="B39" s="159" t="s">
         <v>6</v>
       </c>
       <c r="C39" t="s">
@@ -14724,7 +14726,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B40" s="160"/>
+      <c r="B40" s="159"/>
       <c r="C40" t="s">
         <v>150</v>
       </c>
@@ -14745,7 +14747,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B41" s="160"/>
+      <c r="B41" s="159"/>
       <c r="C41" t="s">
         <v>160</v>
       </c>
@@ -14766,7 +14768,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B42" s="160" t="s">
+      <c r="B42" s="159" t="s">
         <v>7</v>
       </c>
       <c r="C42" t="s">
@@ -14789,7 +14791,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B43" s="160"/>
+      <c r="B43" s="159"/>
       <c r="C43" t="s">
         <v>150</v>
       </c>
@@ -14810,7 +14812,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B44" s="160"/>
+      <c r="B44" s="159"/>
       <c r="C44" t="s">
         <v>160</v>
       </c>
@@ -14831,7 +14833,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B45" s="160" t="s">
+      <c r="B45" s="159" t="s">
         <v>8</v>
       </c>
       <c r="C45" t="s">
@@ -14854,7 +14856,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B46" s="160"/>
+      <c r="B46" s="159"/>
       <c r="C46" t="s">
         <v>150</v>
       </c>
@@ -14875,7 +14877,7 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B47" s="160"/>
+      <c r="B47" s="159"/>
       <c r="C47" t="s">
         <v>160</v>
       </c>
@@ -14896,7 +14898,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B48" s="160" t="s">
+      <c r="B48" s="159" t="s">
         <v>9</v>
       </c>
       <c r="C48" t="s">
@@ -14919,7 +14921,7 @@
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B49" s="160"/>
+      <c r="B49" s="159"/>
       <c r="C49" t="s">
         <v>150</v>
       </c>
@@ -14940,7 +14942,7 @@
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B50" s="160"/>
+      <c r="B50" s="159"/>
       <c r="C50" t="s">
         <v>160</v>
       </c>
@@ -14985,6 +14987,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -14995,11 +15002,6 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -17256,7 +17258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -30022,7 +30024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Removed current expenditure for Zanzibar regions
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/regions/InputForCode_Kaskazini_Pemba.xlsx
+++ b/input_spreadsheets/Tanzania/regions/InputForCode_Kaskazini_Pemba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Tanzania/regions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{95545FE7-8941-4B4F-A69B-31A00933A2F0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{827ECAA1-8FF3-1849-B150-077E842C0B93}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="15540" tabRatio="905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6425,10 +6425,10 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="739" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="739" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="739" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="741">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
@@ -8798,7 +8798,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8820,9 +8820,7 @@
       <c r="A2" s="156" t="s">
         <v>273</v>
       </c>
-      <c r="B2" s="160">
-        <v>65000</v>
-      </c>
+      <c r="B2" s="159"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="156" t="s">
@@ -13926,7 +13924,7 @@
       <c r="A2" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="B2" s="159" t="s">
+      <c r="B2" s="160" t="s">
         <v>72</v>
       </c>
       <c r="C2" t="s">
@@ -13949,7 +13947,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B3" s="159"/>
+      <c r="B3" s="160"/>
       <c r="C3" t="s">
         <v>150</v>
       </c>
@@ -13971,7 +13969,7 @@
       <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B4" s="159"/>
+      <c r="B4" s="160"/>
       <c r="C4" t="s">
         <v>160</v>
       </c>
@@ -13993,7 +13991,7 @@
       <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B5" s="159" t="s">
+      <c r="B5" s="160" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
@@ -14016,7 +14014,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B6" s="159"/>
+      <c r="B6" s="160"/>
       <c r="C6" t="s">
         <v>150</v>
       </c>
@@ -14037,7 +14035,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B7" s="159"/>
+      <c r="B7" s="160"/>
       <c r="C7" t="s">
         <v>160</v>
       </c>
@@ -14058,7 +14056,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B8" s="159" t="s">
+      <c r="B8" s="160" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
@@ -14081,7 +14079,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B9" s="159"/>
+      <c r="B9" s="160"/>
       <c r="C9" t="s">
         <v>150</v>
       </c>
@@ -14102,7 +14100,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B10" s="159"/>
+      <c r="B10" s="160"/>
       <c r="C10" t="s">
         <v>160</v>
       </c>
@@ -14123,7 +14121,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B11" s="159" t="s">
+      <c r="B11" s="160" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
@@ -14146,7 +14144,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B12" s="159"/>
+      <c r="B12" s="160"/>
       <c r="C12" t="s">
         <v>150</v>
       </c>
@@ -14167,7 +14165,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B13" s="159"/>
+      <c r="B13" s="160"/>
       <c r="C13" t="s">
         <v>160</v>
       </c>
@@ -14188,7 +14186,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B14" s="159" t="s">
+      <c r="B14" s="160" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
@@ -14211,7 +14209,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B15" s="159"/>
+      <c r="B15" s="160"/>
       <c r="C15" t="s">
         <v>150</v>
       </c>
@@ -14232,7 +14230,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B16" s="159"/>
+      <c r="B16" s="160"/>
       <c r="C16" t="s">
         <v>160</v>
       </c>
@@ -14286,7 +14284,7 @@
       <c r="A19" s="42" t="s">
         <v>154</v>
       </c>
-      <c r="B19" s="159" t="s">
+      <c r="B19" s="160" t="s">
         <v>72</v>
       </c>
       <c r="C19" t="s">
@@ -14309,7 +14307,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B20" s="159"/>
+      <c r="B20" s="160"/>
       <c r="C20" t="s">
         <v>150</v>
       </c>
@@ -14330,7 +14328,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B21" s="159"/>
+      <c r="B21" s="160"/>
       <c r="C21" t="s">
         <v>160</v>
       </c>
@@ -14351,7 +14349,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B22" s="159" t="s">
+      <c r="B22" s="160" t="s">
         <v>6</v>
       </c>
       <c r="C22" t="s">
@@ -14374,7 +14372,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B23" s="159"/>
+      <c r="B23" s="160"/>
       <c r="C23" t="s">
         <v>150</v>
       </c>
@@ -14395,7 +14393,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B24" s="159"/>
+      <c r="B24" s="160"/>
       <c r="C24" t="s">
         <v>160</v>
       </c>
@@ -14416,7 +14414,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B25" s="159" t="s">
+      <c r="B25" s="160" t="s">
         <v>7</v>
       </c>
       <c r="C25" t="s">
@@ -14439,7 +14437,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B26" s="159"/>
+      <c r="B26" s="160"/>
       <c r="C26" t="s">
         <v>150</v>
       </c>
@@ -14460,7 +14458,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B27" s="159"/>
+      <c r="B27" s="160"/>
       <c r="C27" t="s">
         <v>160</v>
       </c>
@@ -14481,7 +14479,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B28" s="159" t="s">
+      <c r="B28" s="160" t="s">
         <v>8</v>
       </c>
       <c r="C28" t="s">
@@ -14504,7 +14502,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B29" s="159"/>
+      <c r="B29" s="160"/>
       <c r="C29" t="s">
         <v>150</v>
       </c>
@@ -14525,7 +14523,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B30" s="159"/>
+      <c r="B30" s="160"/>
       <c r="C30" t="s">
         <v>160</v>
       </c>
@@ -14546,7 +14544,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B31" s="159" t="s">
+      <c r="B31" s="160" t="s">
         <v>9</v>
       </c>
       <c r="C31" t="s">
@@ -14569,7 +14567,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B32" s="159"/>
+      <c r="B32" s="160"/>
       <c r="C32" t="s">
         <v>150</v>
       </c>
@@ -14590,7 +14588,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B33" s="159"/>
+      <c r="B33" s="160"/>
       <c r="C33" t="s">
         <v>160</v>
       </c>
@@ -14637,7 +14635,7 @@
       <c r="A36" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="B36" s="159" t="s">
+      <c r="B36" s="160" t="s">
         <v>72</v>
       </c>
       <c r="C36" t="s">
@@ -14660,7 +14658,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B37" s="159"/>
+      <c r="B37" s="160"/>
       <c r="C37" t="s">
         <v>150</v>
       </c>
@@ -14681,7 +14679,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B38" s="159"/>
+      <c r="B38" s="160"/>
       <c r="C38" t="s">
         <v>160</v>
       </c>
@@ -14703,7 +14701,7 @@
       <c r="I38" s="38"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B39" s="159" t="s">
+      <c r="B39" s="160" t="s">
         <v>6</v>
       </c>
       <c r="C39" t="s">
@@ -14726,7 +14724,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B40" s="159"/>
+      <c r="B40" s="160"/>
       <c r="C40" t="s">
         <v>150</v>
       </c>
@@ -14747,7 +14745,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B41" s="159"/>
+      <c r="B41" s="160"/>
       <c r="C41" t="s">
         <v>160</v>
       </c>
@@ -14768,7 +14766,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B42" s="159" t="s">
+      <c r="B42" s="160" t="s">
         <v>7</v>
       </c>
       <c r="C42" t="s">
@@ -14791,7 +14789,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B43" s="159"/>
+      <c r="B43" s="160"/>
       <c r="C43" t="s">
         <v>150</v>
       </c>
@@ -14812,7 +14810,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B44" s="159"/>
+      <c r="B44" s="160"/>
       <c r="C44" t="s">
         <v>160</v>
       </c>
@@ -14833,7 +14831,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B45" s="159" t="s">
+      <c r="B45" s="160" t="s">
         <v>8</v>
       </c>
       <c r="C45" t="s">
@@ -14856,7 +14854,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B46" s="159"/>
+      <c r="B46" s="160"/>
       <c r="C46" t="s">
         <v>150</v>
       </c>
@@ -14877,7 +14875,7 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B47" s="159"/>
+      <c r="B47" s="160"/>
       <c r="C47" t="s">
         <v>160</v>
       </c>
@@ -14898,7 +14896,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B48" s="159" t="s">
+      <c r="B48" s="160" t="s">
         <v>9</v>
       </c>
       <c r="C48" t="s">
@@ -14921,7 +14919,7 @@
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B49" s="159"/>
+      <c r="B49" s="160"/>
       <c r="C49" t="s">
         <v>150</v>
       </c>
@@ -14942,7 +14940,7 @@
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B50" s="159"/>
+      <c r="B50" s="160"/>
       <c r="C50" t="s">
         <v>160</v>
       </c>
@@ -14987,11 +14985,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -15002,6 +14995,11 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>